<commit_message>
updates to sentence verification and stroop tasks
</commit_message>
<xml_diff>
--- a/SentenceVerification/stims_set2.xlsx
+++ b/SentenceVerification/stims_set2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ethan/Documents/GitHub/OpenSesame/SentenceVerification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0938F891-0F92-1041-9E74-8DF7E1E2D69C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBDD8369-C32C-9943-A79F-92E69605565F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="10520" yWindow="3440" windowWidth="26440" windowHeight="15440" xr2:uid="{6593727D-1531-3642-BF60-B86A658FA13D}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>P1</t>
   </si>
   <si>
-    <t>A almond is square.</t>
-  </si>
-  <si>
     <t>A chestnut has a shell.</t>
   </si>
   <si>
@@ -97,9 +94,6 @@
     <t>An optometrist has a drill.</t>
   </si>
   <si>
-    <t>An occulist has patients.</t>
-  </si>
-  <si>
     <t>A dentist has fans.</t>
   </si>
   <si>
@@ -190,15 +184,9 @@
     <t>A bedroom is a bedroom.</t>
   </si>
   <si>
-    <t>A mulberry has needles.</t>
-  </si>
-  <si>
     <t>A fir has branches.</t>
   </si>
   <si>
-    <t>A sahuara has lemons.</t>
-  </si>
-  <si>
     <t>An oak has acorns.</t>
   </si>
   <si>
@@ -238,9 +226,6 @@
     <t>Brandy is brandy.</t>
   </si>
   <si>
-    <t>A infantryman has a rocket.</t>
-  </si>
-  <si>
     <t>A sergeant has a uniform.</t>
   </si>
   <si>
@@ -292,9 +277,6 @@
     <t>Beans have protein.</t>
   </si>
   <si>
-    <t>Balogna is gray.</t>
-  </si>
-  <si>
     <t>Bananas are yellow.</t>
   </si>
   <si>
@@ -310,30 +292,18 @@
     <t>Peas are peas.</t>
   </si>
   <si>
-    <t>A jeep has wings.</t>
-  </si>
-  <si>
     <t>A truck has wheels.</t>
   </si>
   <si>
-    <t>A compact is big.</t>
-  </si>
-  <si>
     <t>A limousine is long.</t>
   </si>
   <si>
-    <t>A corvette is an airplane.</t>
-  </si>
-  <si>
     <t>S1.</t>
   </si>
   <si>
     <t>A pecan is a nut.</t>
   </si>
   <si>
-    <t>A ford is a toyota.</t>
-  </si>
-  <si>
     <t>A Chevrolet is a Chevrolet.</t>
   </si>
   <si>
@@ -346,9 +316,6 @@
     <t>Granite is inorganic.</t>
   </si>
   <si>
-    <t>Steak is drinkable,</t>
-  </si>
-  <si>
     <t>Bread is digestable.</t>
   </si>
   <si>
@@ -398,6 +365,39 @@
   </si>
   <si>
     <t>[true_response]</t>
+  </si>
+  <si>
+    <t>A daisy has needles.</t>
+  </si>
+  <si>
+    <t>An infantryman has a rocket.</t>
+  </si>
+  <si>
+    <t>A Jeep has wings.</t>
+  </si>
+  <si>
+    <t>Steak is drinkable.</t>
+  </si>
+  <si>
+    <t>A palm has lemons.</t>
+  </si>
+  <si>
+    <t>Mozarella is gray.</t>
+  </si>
+  <si>
+    <t>A lipstick is big.</t>
+  </si>
+  <si>
+    <t>A Porsche is an airplane.</t>
+  </si>
+  <si>
+    <t>A Ford is a Toyota.</t>
+  </si>
+  <si>
+    <t>An ophthalmologist has patients.</t>
+  </si>
+  <si>
+    <t>An almond is square.</t>
   </si>
 </sst>
 </file>
@@ -751,24 +751,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EFB4AA9-4ADB-3E4D-81D4-F45F8E2A29B3}">
   <dimension ref="A1:D109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="B1" t="s">
-        <v>117</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>118</v>
+        <v>107</v>
       </c>
       <c r="D1" t="s">
-        <v>119</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -779,10 +779,10 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>1</v>
+        <v>121</v>
       </c>
       <c r="D2" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -793,10 +793,10 @@
         <v>0</v>
       </c>
       <c r="C3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -807,10 +807,10 @@
         <v>0</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -821,10 +821,10 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -835,10 +835,10 @@
         <v>0</v>
       </c>
       <c r="C6" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -849,10 +849,10 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -863,10 +863,10 @@
         <v>0</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>111</v>
       </c>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -877,10 +877,10 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -891,10 +891,10 @@
         <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>68</v>
+        <v>112</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -905,10 +905,10 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -919,10 +919,10 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D12" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -933,10 +933,10 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
       <c r="D13" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -944,13 +944,13 @@
         <v>0</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C14" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -958,13 +958,13 @@
         <v>0</v>
       </c>
       <c r="B15" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>114</v>
       </c>
       <c r="D15" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -972,13 +972,13 @@
         <v>0</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C16" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -986,13 +986,13 @@
         <v>0</v>
       </c>
       <c r="B17" t="s">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -1000,13 +1000,13 @@
         <v>0</v>
       </c>
       <c r="B18" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D18" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1014,13 +1014,13 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D19" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1028,13 +1028,13 @@
         <v>0</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D20" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1042,13 +1042,13 @@
         <v>0</v>
       </c>
       <c r="B21" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1056,13 +1056,13 @@
         <v>0</v>
       </c>
       <c r="B22" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D22" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1070,13 +1070,13 @@
         <v>0</v>
       </c>
       <c r="B23" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>54</v>
+        <v>115</v>
       </c>
       <c r="D23" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1084,13 +1084,13 @@
         <v>0</v>
       </c>
       <c r="B24" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1098,13 +1098,13 @@
         <v>0</v>
       </c>
       <c r="B25" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C25" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D25" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1112,13 +1112,13 @@
         <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C26" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D26" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1126,13 +1126,13 @@
         <v>0</v>
       </c>
       <c r="B27" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C27" t="s">
-        <v>86</v>
+        <v>116</v>
       </c>
       <c r="D27" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1140,13 +1140,13 @@
         <v>0</v>
       </c>
       <c r="B28" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C28" t="s">
-        <v>94</v>
+        <v>117</v>
       </c>
       <c r="D28" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1154,13 +1154,13 @@
         <v>0</v>
       </c>
       <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29" t="s">
         <v>6</v>
       </c>
-      <c r="C29" t="s">
-        <v>7</v>
-      </c>
       <c r="D29" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1168,13 +1168,13 @@
         <v>0</v>
       </c>
       <c r="B30" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C30" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D30" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1182,13 +1182,13 @@
         <v>0</v>
       </c>
       <c r="B31" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D31" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1196,13 +1196,13 @@
         <v>0</v>
       </c>
       <c r="B32" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C32" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D32" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1210,13 +1210,13 @@
         <v>0</v>
       </c>
       <c r="B33" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D33" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1224,13 +1224,13 @@
         <v>0</v>
       </c>
       <c r="B34" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D34" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1238,13 +1238,13 @@
         <v>0</v>
       </c>
       <c r="B35" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C35" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D35" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1252,13 +1252,13 @@
         <v>0</v>
       </c>
       <c r="B36" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C36" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D36" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1266,13 +1266,13 @@
         <v>0</v>
       </c>
       <c r="B37" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C37" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D37" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1280,13 +1280,13 @@
         <v>0</v>
       </c>
       <c r="B38" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C38" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1294,13 +1294,13 @@
         <v>0</v>
       </c>
       <c r="B39" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1308,13 +1308,13 @@
         <v>0</v>
       </c>
       <c r="B40" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C40" t="s">
-        <v>96</v>
+        <v>118</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1322,13 +1322,13 @@
         <v>0</v>
       </c>
       <c r="B41" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C41" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="D41" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1336,13 +1336,13 @@
         <v>0</v>
       </c>
       <c r="B42" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C42" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="D42" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1350,13 +1350,13 @@
         <v>0</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C43" t="s">
-        <v>113</v>
+        <v>102</v>
       </c>
       <c r="D43" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1364,13 +1364,13 @@
         <v>0</v>
       </c>
       <c r="B44" t="s">
+        <v>8</v>
+      </c>
+      <c r="C44" t="s">
         <v>9</v>
       </c>
-      <c r="C44" t="s">
-        <v>10</v>
-      </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1378,13 +1378,13 @@
         <v>0</v>
       </c>
       <c r="B45" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1392,13 +1392,13 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D46" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1406,13 +1406,13 @@
         <v>0</v>
       </c>
       <c r="B47" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D47" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1420,13 +1420,13 @@
         <v>0</v>
       </c>
       <c r="B48" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D48" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1434,13 +1434,13 @@
         <v>0</v>
       </c>
       <c r="B49" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1448,13 +1448,13 @@
         <v>0</v>
       </c>
       <c r="B50" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="D50" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1462,13 +1462,13 @@
         <v>0</v>
       </c>
       <c r="B51" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="D51" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1476,13 +1476,13 @@
         <v>0</v>
       </c>
       <c r="B52" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D52" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1490,13 +1490,13 @@
         <v>0</v>
       </c>
       <c r="B53" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D53" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1504,13 +1504,13 @@
         <v>0</v>
       </c>
       <c r="B54" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="D54" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1518,13 +1518,13 @@
         <v>0</v>
       </c>
       <c r="B55" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>99</v>
+        <v>119</v>
       </c>
       <c r="D55" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1535,10 +1535,10 @@
         <v>0</v>
       </c>
       <c r="C56" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D56" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1549,10 +1549,10 @@
         <v>0</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D57" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1563,10 +1563,10 @@
         <v>0</v>
       </c>
       <c r="C58" t="s">
-        <v>21</v>
+        <v>120</v>
       </c>
       <c r="D58" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1577,10 +1577,10 @@
         <v>0</v>
       </c>
       <c r="C59" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D59" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1591,10 +1591,10 @@
         <v>0</v>
       </c>
       <c r="C60" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D60" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1605,10 +1605,10 @@
         <v>0</v>
       </c>
       <c r="C61" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D61" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1619,10 +1619,10 @@
         <v>0</v>
       </c>
       <c r="C62" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D62" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1633,10 +1633,10 @@
         <v>0</v>
       </c>
       <c r="C63" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D63" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1647,10 +1647,10 @@
         <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D64" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1661,10 +1661,10 @@
         <v>0</v>
       </c>
       <c r="C65" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D65" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1675,10 +1675,10 @@
         <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="D66" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1689,10 +1689,10 @@
         <v>0</v>
       </c>
       <c r="C67" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="D67" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -1700,13 +1700,13 @@
         <v>1</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C68" t="s">
-        <v>103</v>
+        <v>93</v>
       </c>
       <c r="D68" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1714,13 +1714,13 @@
         <v>1</v>
       </c>
       <c r="B69" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="D69" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
@@ -1728,13 +1728,13 @@
         <v>1</v>
       </c>
       <c r="B70" t="s">
-        <v>101</v>
+        <v>91</v>
       </c>
       <c r="C70" t="s">
-        <v>107</v>
+        <v>96</v>
       </c>
       <c r="D70" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
@@ -1742,13 +1742,13 @@
         <v>1</v>
       </c>
       <c r="B71" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C71" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D71" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1756,13 +1756,13 @@
         <v>1</v>
       </c>
       <c r="B72" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D72" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1770,13 +1770,13 @@
         <v>1</v>
       </c>
       <c r="B73" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D73" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1784,13 +1784,13 @@
         <v>1</v>
       </c>
       <c r="B74" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C74" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D74" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -1798,13 +1798,13 @@
         <v>1</v>
       </c>
       <c r="B75" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C75" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D75" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -1812,13 +1812,13 @@
         <v>1</v>
       </c>
       <c r="B76" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C76" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D76" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -1826,13 +1826,13 @@
         <v>1</v>
       </c>
       <c r="B77" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C77" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D77" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -1840,13 +1840,13 @@
         <v>1</v>
       </c>
       <c r="B78" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="D78" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -1854,13 +1854,13 @@
         <v>1</v>
       </c>
       <c r="B79" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C79" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D79" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -1868,13 +1868,13 @@
         <v>1</v>
       </c>
       <c r="B80" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="D80" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -1882,13 +1882,13 @@
         <v>1</v>
       </c>
       <c r="B81" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C81" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
       <c r="D81" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -1896,13 +1896,13 @@
         <v>1</v>
       </c>
       <c r="B82" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C82" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D82" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -1910,13 +1910,13 @@
         <v>1</v>
       </c>
       <c r="B83" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C83" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D83" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -1924,13 +1924,13 @@
         <v>1</v>
       </c>
       <c r="B84" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C84" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D84" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -1938,13 +1938,13 @@
         <v>1</v>
       </c>
       <c r="B85" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C85" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D85" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -1952,13 +1952,13 @@
         <v>1</v>
       </c>
       <c r="B86" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C86" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D86" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -1966,13 +1966,13 @@
         <v>1</v>
       </c>
       <c r="B87" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C87" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D87" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -1980,13 +1980,13 @@
         <v>1</v>
       </c>
       <c r="B88" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C88" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D88" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -1994,13 +1994,13 @@
         <v>1</v>
       </c>
       <c r="B89" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C89" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D89" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
@@ -2008,13 +2008,13 @@
         <v>1</v>
       </c>
       <c r="B90" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C90" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="D90" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2022,13 +2022,13 @@
         <v>1</v>
       </c>
       <c r="B91" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C91" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D91" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
@@ -2036,13 +2036,13 @@
         <v>1</v>
       </c>
       <c r="B92" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C92" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D92" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
@@ -2050,13 +2050,13 @@
         <v>1</v>
       </c>
       <c r="B93" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C93" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="D93" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
@@ -2064,13 +2064,13 @@
         <v>1</v>
       </c>
       <c r="B94" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C94" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="D94" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
@@ -2078,13 +2078,13 @@
         <v>1</v>
       </c>
       <c r="B95" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C95" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="D95" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2092,13 +2092,13 @@
         <v>1</v>
       </c>
       <c r="B96" t="s">
-        <v>108</v>
+        <v>97</v>
       </c>
       <c r="C96" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="D96" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2106,13 +2106,13 @@
         <v>1</v>
       </c>
       <c r="B97" t="s">
-        <v>114</v>
+        <v>103</v>
       </c>
       <c r="C97" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="D97" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2120,13 +2120,13 @@
         <v>1</v>
       </c>
       <c r="B98" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C98" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D98" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2134,13 +2134,13 @@
         <v>1</v>
       </c>
       <c r="B99" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C99" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D99" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2148,13 +2148,13 @@
         <v>1</v>
       </c>
       <c r="B100" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D100" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2162,13 +2162,13 @@
         <v>1</v>
       </c>
       <c r="B101" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C101" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D101" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2176,13 +2176,13 @@
         <v>1</v>
       </c>
       <c r="B102" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C102" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D102" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2190,13 +2190,13 @@
         <v>1</v>
       </c>
       <c r="B103" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C103" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D103" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2204,13 +2204,13 @@
         <v>1</v>
       </c>
       <c r="B104" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C104" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="D104" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2218,13 +2218,13 @@
         <v>1</v>
       </c>
       <c r="B105" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C105" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D105" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2232,13 +2232,13 @@
         <v>1</v>
       </c>
       <c r="B106" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C106" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D106" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2246,13 +2246,13 @@
         <v>1</v>
       </c>
       <c r="B107" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C107" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D107" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2260,13 +2260,13 @@
         <v>1</v>
       </c>
       <c r="B108" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C108" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="D108" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2274,13 +2274,13 @@
         <v>1</v>
       </c>
       <c r="B109" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C109" t="s">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="D109" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
   </sheetData>

</xml_diff>